<commit_message>
Reduce near-term renovations to fit MEPS schedule; flip sign on BRESaC energy savings
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BRESaC/Bldg Retrofitting E Savings and Costs.xlsx
+++ b/InputData/bldgs/BRESaC/Bldg Retrofitting E Savings and Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\bldgs\BRESaC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\bldgs\BRESaC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE709BDC-4715-4232-9438-A8082CDA6542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE871DA-E75B-4A5D-8918-0BDE2A174455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5880" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33105" yWindow="3045" windowWidth="18765" windowHeight="12960" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -1974,7 +1974,7 @@
   <dimension ref="A1:AO61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ59" sqref="AJ59"/>
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2742,159 +2742,159 @@
         <v>103</v>
       </c>
       <c r="C8">
-        <f>SUM(C4:C7)</f>
+        <f t="shared" ref="C8:AO8" si="0">SUM(C4:C7)</f>
         <v>535.38849971629782</v>
       </c>
       <c r="D8">
-        <f>SUM(D4:D7)</f>
+        <f t="shared" si="0"/>
         <v>538.91909208493371</v>
       </c>
       <c r="E8">
-        <f>SUM(E4:E7)</f>
+        <f t="shared" si="0"/>
         <v>543.29009945444216</v>
       </c>
       <c r="F8">
-        <f>SUM(F4:F7)</f>
+        <f t="shared" si="0"/>
         <v>546.7204540729299</v>
       </c>
       <c r="G8">
-        <f>SUM(G4:G7)</f>
+        <f t="shared" si="0"/>
         <v>549.28457075994061</v>
       </c>
       <c r="H8">
-        <f>SUM(H4:H7)</f>
+        <f t="shared" si="0"/>
         <v>555.29806501142377</v>
       </c>
       <c r="I8">
-        <f>SUM(I4:I7)</f>
+        <f t="shared" si="0"/>
         <v>555.23738279998452</v>
       </c>
       <c r="J8">
-        <f>SUM(J4:J7)</f>
+        <f t="shared" si="0"/>
         <v>556.8732893557135</v>
       </c>
       <c r="K8">
-        <f>SUM(K4:K7)</f>
+        <f t="shared" si="0"/>
         <v>554.0278424429348</v>
       </c>
       <c r="L8">
-        <f>SUM(L4:L7)</f>
+        <f t="shared" si="0"/>
         <v>550.56783194589127</v>
       </c>
       <c r="M8">
-        <f>SUM(M4:M7)</f>
+        <f t="shared" si="0"/>
         <v>548.37493747815552</v>
       </c>
       <c r="N8">
-        <f>SUM(N4:N7)</f>
+        <f t="shared" si="0"/>
         <v>544.99710395265561</v>
       </c>
       <c r="O8">
-        <f>SUM(O4:O7)</f>
+        <f t="shared" si="0"/>
         <v>542.18381433119214</v>
       </c>
       <c r="P8">
-        <f>SUM(P4:P7)</f>
+        <f t="shared" si="0"/>
         <v>541.19772315441071</v>
       </c>
       <c r="Q8">
-        <f>SUM(Q4:Q7)</f>
+        <f t="shared" si="0"/>
         <v>538.82420337273811</v>
       </c>
       <c r="R8">
-        <f>SUM(R4:R7)</f>
+        <f t="shared" si="0"/>
         <v>536.90178990782317</v>
       </c>
       <c r="S8">
-        <f>SUM(S4:S7)</f>
+        <f t="shared" si="0"/>
         <v>535.63580402753439</v>
       </c>
       <c r="T8">
-        <f>SUM(T4:T7)</f>
+        <f t="shared" si="0"/>
         <v>534.08076165051421</v>
       </c>
       <c r="U8" s="1">
-        <f>SUM(U4:U7)</f>
+        <f t="shared" si="0"/>
         <v>532.56628229455873</v>
       </c>
       <c r="V8">
-        <f>SUM(V4:V7)</f>
+        <f t="shared" si="0"/>
         <v>530.03536899271614</v>
       </c>
       <c r="W8">
-        <f>SUM(W4:W7)</f>
+        <f t="shared" si="0"/>
         <v>527.97466379714001</v>
       </c>
       <c r="X8">
-        <f>SUM(X4:X7)</f>
+        <f t="shared" si="0"/>
         <v>525.71982441055434</v>
       </c>
       <c r="Y8">
-        <f>SUM(Y4:Y7)</f>
+        <f t="shared" si="0"/>
         <v>523.36160076869703</v>
       </c>
       <c r="Z8" s="1">
-        <f>SUM(Z4:Z7)</f>
+        <f t="shared" si="0"/>
         <v>521.23944186205233</v>
       </c>
       <c r="AA8">
-        <f>SUM(AA4:AA7)</f>
+        <f t="shared" si="0"/>
         <v>518.47030630453719</v>
       </c>
       <c r="AB8">
-        <f>SUM(AB4:AB7)</f>
+        <f t="shared" si="0"/>
         <v>516.16058222964398</v>
       </c>
       <c r="AC8">
-        <f>SUM(AC4:AC7)</f>
+        <f t="shared" si="0"/>
         <v>513.29215901858265</v>
       </c>
       <c r="AD8">
-        <f>SUM(AD4:AD7)</f>
+        <f t="shared" si="0"/>
         <v>510.637454684668</v>
       </c>
       <c r="AE8">
-        <f>SUM(AE4:AE7)</f>
+        <f t="shared" si="0"/>
         <v>508.01872211266925</v>
       </c>
       <c r="AF8">
-        <f>SUM(AF4:AF7)</f>
+        <f t="shared" si="0"/>
         <v>505.17939508129223</v>
       </c>
       <c r="AG8">
-        <f>SUM(AG4:AG7)</f>
+        <f t="shared" si="0"/>
         <v>502.91324698355646</v>
       </c>
       <c r="AH8">
-        <f>SUM(AH4:AH7)</f>
+        <f t="shared" si="0"/>
         <v>500.24822351918971</v>
       </c>
       <c r="AI8">
-        <f>SUM(AI4:AI7)</f>
+        <f t="shared" si="0"/>
         <v>497.58427326763183</v>
       </c>
       <c r="AJ8">
-        <f>SUM(AJ4:AJ7)</f>
+        <f t="shared" si="0"/>
         <v>495.3581814188214</v>
       </c>
       <c r="AK8">
-        <f>SUM(AK4:AK7)</f>
+        <f t="shared" si="0"/>
         <v>492.23946501319421</v>
       </c>
       <c r="AL8">
-        <f>SUM(AL4:AL7)</f>
+        <f t="shared" si="0"/>
         <v>489.56765175759978</v>
       </c>
       <c r="AM8">
-        <f>SUM(AM4:AM7)</f>
+        <f t="shared" si="0"/>
         <v>486.76362275995768</v>
       </c>
       <c r="AN8">
-        <f>SUM(AN4:AN7)</f>
+        <f t="shared" si="0"/>
         <v>485.02267708619758</v>
       </c>
       <c r="AO8">
-        <f>SUM(AO4:AO7)</f>
+        <f t="shared" si="0"/>
         <v>482.66195114430155</v>
       </c>
     </row>
@@ -3555,159 +3555,159 @@
         <v>102</v>
       </c>
       <c r="C18">
-        <f>C3*10^9/C11</f>
+        <f t="shared" ref="C18:AO18" si="1">C3*10^9/C11</f>
         <v>168.62175118580225</v>
       </c>
       <c r="D18">
-        <f>D3*10^9/D11</f>
+        <f t="shared" si="1"/>
         <v>166.9945113004085</v>
       </c>
       <c r="E18">
-        <f>E3*10^9/E11</f>
+        <f t="shared" si="1"/>
         <v>165.43423148147218</v>
       </c>
       <c r="F18">
-        <f>F3*10^9/F11</f>
+        <f t="shared" si="1"/>
         <v>163.8509505683146</v>
       </c>
       <c r="G18">
-        <f>G3*10^9/G11</f>
+        <f t="shared" si="1"/>
         <v>162.27688026102663</v>
       </c>
       <c r="H18">
-        <f>H3*10^9/H11</f>
+        <f t="shared" si="1"/>
         <v>160.68972603784371</v>
       </c>
       <c r="I18">
-        <f>I3*10^9/I11</f>
+        <f t="shared" si="1"/>
         <v>159.09776882563872</v>
       </c>
       <c r="J18">
-        <f>J3*10^9/J11</f>
+        <f t="shared" si="1"/>
         <v>157.53088991526732</v>
       </c>
       <c r="K18">
-        <f>K3*10^9/K11</f>
+        <f t="shared" si="1"/>
         <v>155.91188201082332</v>
       </c>
       <c r="L18">
-        <f>L3*10^9/L11</f>
+        <f t="shared" si="1"/>
         <v>154.09821940798636</v>
       </c>
       <c r="M18">
-        <f>M3*10^9/M11</f>
+        <f t="shared" si="1"/>
         <v>152.34143187723879</v>
       </c>
       <c r="N18">
-        <f>N3*10^9/N11</f>
+        <f t="shared" si="1"/>
         <v>150.4704948167217</v>
       </c>
       <c r="O18">
-        <f>O3*10^9/O11</f>
+        <f t="shared" si="1"/>
         <v>148.61925890075349</v>
       </c>
       <c r="P18">
-        <f>P3*10^9/P11</f>
+        <f t="shared" si="1"/>
         <v>146.7646465932969</v>
       </c>
       <c r="Q18">
-        <f>Q3*10^9/Q11</f>
+        <f t="shared" si="1"/>
         <v>145.01359112828794</v>
       </c>
       <c r="R18">
-        <f>R3*10^9/R11</f>
+        <f t="shared" si="1"/>
         <v>143.21120121244996</v>
       </c>
       <c r="S18">
-        <f>S3*10^9/S11</f>
+        <f t="shared" si="1"/>
         <v>141.5033650262497</v>
       </c>
       <c r="T18">
-        <f>T3*10^9/T11</f>
+        <f t="shared" si="1"/>
         <v>139.75052809234421</v>
       </c>
       <c r="U18">
-        <f>U3*10^9/U11</f>
+        <f t="shared" si="1"/>
         <v>138.01287769782709</v>
       </c>
       <c r="V18">
-        <f>V3*10^9/V11</f>
+        <f t="shared" si="1"/>
         <v>136.31408197291594</v>
       </c>
       <c r="W18">
-        <f>W3*10^9/W11</f>
+        <f t="shared" si="1"/>
         <v>134.5842195937625</v>
       </c>
       <c r="X18">
-        <f>X3*10^9/X11</f>
+        <f t="shared" si="1"/>
         <v>132.94379561237685</v>
       </c>
       <c r="Y18">
-        <f>Y3*10^9/Y11</f>
+        <f t="shared" si="1"/>
         <v>131.3477708677961</v>
       </c>
       <c r="Z18">
-        <f>Z3*10^9/Z11</f>
+        <f t="shared" si="1"/>
         <v>129.78016241334447</v>
       </c>
       <c r="AA18">
-        <f>AA3*10^9/AA11</f>
+        <f t="shared" si="1"/>
         <v>128.18788507830405</v>
       </c>
       <c r="AB18">
-        <f>AB3*10^9/AB11</f>
+        <f t="shared" si="1"/>
         <v>126.66140387705178</v>
       </c>
       <c r="AC18">
-        <f>AC3*10^9/AC11</f>
+        <f t="shared" si="1"/>
         <v>125.18166185578141</v>
       </c>
       <c r="AD18">
-        <f>AD3*10^9/AD11</f>
+        <f t="shared" si="1"/>
         <v>123.75148228042389</v>
       </c>
       <c r="AE18">
-        <f>AE3*10^9/AE11</f>
+        <f t="shared" si="1"/>
         <v>122.34265098337366</v>
       </c>
       <c r="AF18">
-        <f>AF3*10^9/AF11</f>
+        <f t="shared" si="1"/>
         <v>120.94876194211994</v>
       </c>
       <c r="AG18">
-        <f>AG3*10^9/AG11</f>
+        <f t="shared" si="1"/>
         <v>119.60288703342948</v>
       </c>
       <c r="AH18">
-        <f>AH3*10^9/AH11</f>
+        <f t="shared" si="1"/>
         <v>118.22541471891374</v>
       </c>
       <c r="AI18">
-        <f>AI3*10^9/AI11</f>
+        <f t="shared" si="1"/>
         <v>116.91113172916236</v>
       </c>
       <c r="AJ18">
-        <f>AJ3*10^9/AJ11</f>
+        <f t="shared" si="1"/>
         <v>115.65380861387032</v>
       </c>
       <c r="AK18">
-        <f>AK3*10^9/AK11</f>
+        <f t="shared" si="1"/>
         <v>114.42493972360802</v>
       </c>
       <c r="AL18">
-        <f>AL3*10^9/AL11</f>
+        <f t="shared" si="1"/>
         <v>113.19465982743949</v>
       </c>
       <c r="AM18">
-        <f>AM3*10^9/AM11</f>
+        <f t="shared" si="1"/>
         <v>111.92705918333725</v>
       </c>
       <c r="AN18">
-        <f>AN3*10^9/AN11</f>
+        <f t="shared" si="1"/>
         <v>110.77293338240585</v>
       </c>
       <c r="AO18">
-        <f>AO3*10^9/AO11</f>
+        <f t="shared" si="1"/>
         <v>109.63665906731201</v>
       </c>
     </row>
@@ -3716,159 +3716,159 @@
         <v>98</v>
       </c>
       <c r="C19">
-        <f>C4*10^9/C12</f>
+        <f t="shared" ref="C19:AO19" si="2">C4*10^9/C12</f>
         <v>167.75093034392182</v>
       </c>
       <c r="D19">
-        <f>D4*10^9/D12</f>
+        <f t="shared" si="2"/>
         <v>167.06374031943508</v>
       </c>
       <c r="E19">
-        <f>E4*10^9/E12</f>
+        <f t="shared" si="2"/>
         <v>166.3794817931558</v>
       </c>
       <c r="F19">
-        <f>F4*10^9/F12</f>
+        <f t="shared" si="2"/>
         <v>165.71867705556181</v>
       </c>
       <c r="G19">
-        <f>G4*10^9/G12</f>
+        <f t="shared" si="2"/>
         <v>164.92025375076702</v>
       </c>
       <c r="H19">
-        <f>H4*10^9/H12</f>
+        <f t="shared" si="2"/>
         <v>164.13746927453522</v>
       </c>
       <c r="I19">
-        <f>I4*10^9/I12</f>
+        <f t="shared" si="2"/>
         <v>163.31672014377054</v>
       </c>
       <c r="J19">
-        <f>J4*10^9/J12</f>
+        <f t="shared" si="2"/>
         <v>162.4892991373745</v>
       </c>
       <c r="K19">
-        <f>K4*10^9/K12</f>
+        <f t="shared" si="2"/>
         <v>161.57178394835319</v>
       </c>
       <c r="L19">
-        <f>L4*10^9/L12</f>
+        <f t="shared" si="2"/>
         <v>160.50126694997797</v>
       </c>
       <c r="M19">
-        <f>M4*10^9/M12</f>
+        <f t="shared" si="2"/>
         <v>159.38689136080725</v>
       </c>
       <c r="N19">
-        <f>N4*10^9/N12</f>
+        <f t="shared" si="2"/>
         <v>158.24363522143247</v>
       </c>
       <c r="O19">
-        <f>O4*10^9/O12</f>
+        <f t="shared" si="2"/>
         <v>156.93830780801338</v>
       </c>
       <c r="P19">
-        <f>P4*10^9/P12</f>
+        <f t="shared" si="2"/>
         <v>155.68148459693489</v>
       </c>
       <c r="Q19">
-        <f>Q4*10^9/Q12</f>
+        <f t="shared" si="2"/>
         <v>154.41445977263604</v>
       </c>
       <c r="R19">
-        <f>R4*10^9/R12</f>
+        <f t="shared" si="2"/>
         <v>153.1897353259439</v>
       </c>
       <c r="S19">
-        <f>S4*10^9/S12</f>
+        <f t="shared" si="2"/>
         <v>151.87381686912195</v>
       </c>
       <c r="T19">
-        <f>T4*10^9/T12</f>
+        <f t="shared" si="2"/>
         <v>150.54368836347413</v>
       </c>
       <c r="U19">
-        <f>U4*10^9/U12</f>
+        <f t="shared" si="2"/>
         <v>149.18970688344487</v>
       </c>
       <c r="V19">
-        <f>V4*10^9/V12</f>
+        <f t="shared" si="2"/>
         <v>147.895261507491</v>
       </c>
       <c r="W19">
-        <f>W4*10^9/W12</f>
+        <f t="shared" si="2"/>
         <v>146.51690746572953</v>
       </c>
       <c r="X19">
-        <f>X4*10^9/X12</f>
+        <f t="shared" si="2"/>
         <v>145.19238325810184</v>
       </c>
       <c r="Y19">
-        <f>Y4*10^9/Y12</f>
+        <f t="shared" si="2"/>
         <v>143.90501569157624</v>
       </c>
       <c r="Z19">
-        <f>Z4*10^9/Z12</f>
+        <f t="shared" si="2"/>
         <v>142.57571834167808</v>
       </c>
       <c r="AA19">
-        <f>AA4*10^9/AA12</f>
+        <f t="shared" si="2"/>
         <v>141.26927912096835</v>
       </c>
       <c r="AB19">
-        <f>AB4*10^9/AB12</f>
+        <f t="shared" si="2"/>
         <v>140.01253797730848</v>
       </c>
       <c r="AC19">
-        <f>AC4*10^9/AC12</f>
+        <f t="shared" si="2"/>
         <v>138.75510188434779</v>
       </c>
       <c r="AD19">
-        <f>AD4*10^9/AD12</f>
+        <f t="shared" si="2"/>
         <v>137.49662197851816</v>
       </c>
       <c r="AE19">
-        <f>AE4*10^9/AE12</f>
+        <f t="shared" si="2"/>
         <v>136.2747134211865</v>
       </c>
       <c r="AF19">
-        <f>AF4*10^9/AF12</f>
+        <f t="shared" si="2"/>
         <v>135.02823615071475</v>
       </c>
       <c r="AG19">
-        <f>AG4*10^9/AG12</f>
+        <f t="shared" si="2"/>
         <v>133.84349014771186</v>
       </c>
       <c r="AH19">
-        <f>AH4*10^9/AH12</f>
+        <f t="shared" si="2"/>
         <v>132.57320184420414</v>
       </c>
       <c r="AI19">
-        <f>AI4*10^9/AI12</f>
+        <f t="shared" si="2"/>
         <v>131.3364381605916</v>
       </c>
       <c r="AJ19">
-        <f>AJ4*10^9/AJ12</f>
+        <f t="shared" si="2"/>
         <v>130.06001964785651</v>
       </c>
       <c r="AK19">
-        <f>AK4*10^9/AK12</f>
+        <f t="shared" si="2"/>
         <v>128.76938643856352</v>
       </c>
       <c r="AL19">
-        <f>AL4*10^9/AL12</f>
+        <f t="shared" si="2"/>
         <v>127.52316053011032</v>
       </c>
       <c r="AM19">
-        <f>AM4*10^9/AM12</f>
+        <f t="shared" si="2"/>
         <v>126.33639054278282</v>
       </c>
       <c r="AN19">
-        <f>AN4*10^9/AN12</f>
+        <f t="shared" si="2"/>
         <v>125.11168459156335</v>
       </c>
       <c r="AO19">
-        <f>AO4*10^9/AO12</f>
+        <f t="shared" si="2"/>
         <v>123.91474517171322</v>
       </c>
     </row>
@@ -3877,159 +3877,159 @@
         <v>99</v>
       </c>
       <c r="C20">
-        <f>C5*10^9/C13</f>
+        <f t="shared" ref="C20:AO20" si="3">C5*10^9/C13</f>
         <v>122.70453681200028</v>
       </c>
       <c r="D20">
-        <f>D5*10^9/D13</f>
+        <f t="shared" si="3"/>
         <v>122.56550531073073</v>
       </c>
       <c r="E20">
-        <f>E5*10^9/E13</f>
+        <f t="shared" si="3"/>
         <v>122.40862990417223</v>
       </c>
       <c r="F20">
-        <f>F5*10^9/F13</f>
+        <f t="shared" si="3"/>
         <v>122.23735270249193</v>
       </c>
       <c r="G20">
-        <f>G5*10^9/G13</f>
+        <f t="shared" si="3"/>
         <v>122.04983207249253</v>
       </c>
       <c r="H20">
-        <f>H5*10^9/H13</f>
+        <f t="shared" si="3"/>
         <v>121.83527251699131</v>
       </c>
       <c r="I20">
-        <f>I5*10^9/I13</f>
+        <f t="shared" si="3"/>
         <v>121.61107441160028</v>
       </c>
       <c r="J20">
-        <f>J5*10^9/J13</f>
+        <f t="shared" si="3"/>
         <v>121.395335541745</v>
       </c>
       <c r="K20">
-        <f>K5*10^9/K13</f>
+        <f t="shared" si="3"/>
         <v>121.14547017245391</v>
       </c>
       <c r="L20">
-        <f>L5*10^9/L13</f>
+        <f t="shared" si="3"/>
         <v>120.80303734583964</v>
       </c>
       <c r="M20">
-        <f>M5*10^9/M13</f>
+        <f t="shared" si="3"/>
         <v>120.45364555649762</v>
       </c>
       <c r="N20">
-        <f>N5*10^9/N13</f>
+        <f t="shared" si="3"/>
         <v>120.0068665728872</v>
       </c>
       <c r="O20">
-        <f>O5*10^9/O13</f>
+        <f t="shared" si="3"/>
         <v>119.48960139343785</v>
       </c>
       <c r="P20">
-        <f>P5*10^9/P13</f>
+        <f t="shared" si="3"/>
         <v>118.99349843758522</v>
       </c>
       <c r="Q20">
-        <f>Q5*10^9/Q13</f>
+        <f t="shared" si="3"/>
         <v>118.53458485308147</v>
       </c>
       <c r="R20">
-        <f>R5*10^9/R13</f>
+        <f t="shared" si="3"/>
         <v>118.07685839911022</v>
       </c>
       <c r="S20">
-        <f>S5*10^9/S13</f>
+        <f t="shared" si="3"/>
         <v>117.63727138961781</v>
       </c>
       <c r="T20">
-        <f>T5*10^9/T13</f>
+        <f t="shared" si="3"/>
         <v>117.19381027873084</v>
       </c>
       <c r="U20">
-        <f>U5*10^9/U13</f>
+        <f t="shared" si="3"/>
         <v>116.79143444539262</v>
       </c>
       <c r="V20">
-        <f>V5*10^9/V13</f>
+        <f t="shared" si="3"/>
         <v>116.36007338929809</v>
       </c>
       <c r="W20">
-        <f>W5*10^9/W13</f>
+        <f t="shared" si="3"/>
         <v>115.91803167621546</v>
       </c>
       <c r="X20">
-        <f>X5*10^9/X13</f>
+        <f t="shared" si="3"/>
         <v>115.4964176570504</v>
       </c>
       <c r="Y20">
-        <f>Y5*10^9/Y13</f>
+        <f t="shared" si="3"/>
         <v>115.09723882765341</v>
       </c>
       <c r="Z20">
-        <f>Z5*10^9/Z13</f>
+        <f t="shared" si="3"/>
         <v>114.70164341889149</v>
       </c>
       <c r="AA20">
-        <f>AA5*10^9/AA13</f>
+        <f t="shared" si="3"/>
         <v>114.33015839973854</v>
       </c>
       <c r="AB20">
-        <f>AB5*10^9/AB13</f>
+        <f t="shared" si="3"/>
         <v>113.89901465552182</v>
       </c>
       <c r="AC20">
-        <f>AC5*10^9/AC13</f>
+        <f t="shared" si="3"/>
         <v>113.49253468693374</v>
       </c>
       <c r="AD20">
-        <f>AD5*10^9/AD13</f>
+        <f t="shared" si="3"/>
         <v>113.07948566129971</v>
       </c>
       <c r="AE20">
-        <f>AE5*10^9/AE13</f>
+        <f t="shared" si="3"/>
         <v>112.70402317073413</v>
       </c>
       <c r="AF20">
-        <f>AF5*10^9/AF13</f>
+        <f t="shared" si="3"/>
         <v>112.28024410882037</v>
       </c>
       <c r="AG20">
-        <f>AG5*10^9/AG13</f>
+        <f t="shared" si="3"/>
         <v>111.88698710414486</v>
       </c>
       <c r="AH20">
-        <f>AH5*10^9/AH13</f>
+        <f t="shared" si="3"/>
         <v>111.505714041186</v>
       </c>
       <c r="AI20">
-        <f>AI5*10^9/AI13</f>
+        <f t="shared" si="3"/>
         <v>111.14113644736447</v>
       </c>
       <c r="AJ20">
-        <f>AJ5*10^9/AJ13</f>
+        <f t="shared" si="3"/>
         <v>110.77438119966367</v>
       </c>
       <c r="AK20">
-        <f>AK5*10^9/AK13</f>
+        <f t="shared" si="3"/>
         <v>110.3515686748438</v>
       </c>
       <c r="AL20">
-        <f>AL5*10^9/AL13</f>
+        <f t="shared" si="3"/>
         <v>109.91216577872498</v>
       </c>
       <c r="AM20">
-        <f>AM5*10^9/AM13</f>
+        <f t="shared" si="3"/>
         <v>109.49895603153306</v>
       </c>
       <c r="AN20">
-        <f>AN5*10^9/AN13</f>
+        <f t="shared" si="3"/>
         <v>109.08589357219418</v>
       </c>
       <c r="AO20">
-        <f>AO5*10^9/AO13</f>
+        <f t="shared" si="3"/>
         <v>108.67869702891251</v>
       </c>
     </row>
@@ -4038,159 +4038,159 @@
         <v>100</v>
       </c>
       <c r="C21" t="e">
-        <f>C6*10^9/C14</f>
+        <f t="shared" ref="C21:AO21" si="4">C6*10^9/C14</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D21">
-        <f>D6*10^9/D14</f>
+        <f t="shared" si="4"/>
         <v>66.835522982403717</v>
       </c>
       <c r="E21">
-        <f>E6*10^9/E14</f>
+        <f t="shared" si="4"/>
         <v>69.484328084077873</v>
       </c>
       <c r="F21">
-        <f>F6*10^9/F14</f>
+        <f t="shared" si="4"/>
         <v>70.332015718093601</v>
       </c>
       <c r="G21">
-        <f>G6*10^9/G14</f>
+        <f t="shared" si="4"/>
         <v>69.69796486936707</v>
       </c>
       <c r="H21">
-        <f>H6*10^9/H14</f>
+        <f t="shared" si="4"/>
         <v>69.557093392200358</v>
       </c>
       <c r="I21">
-        <f>I6*10^9/I14</f>
+        <f t="shared" si="4"/>
         <v>69.75464195017905</v>
       </c>
       <c r="J21">
-        <f>J6*10^9/J14</f>
+        <f t="shared" si="4"/>
         <v>70.288610388889069</v>
       </c>
       <c r="K21">
-        <f>K6*10^9/K14</f>
+        <f t="shared" si="4"/>
         <v>69.611129053235558</v>
       </c>
       <c r="L21">
-        <f>L6*10^9/L14</f>
+        <f t="shared" si="4"/>
         <v>69.585875259841387</v>
       </c>
       <c r="M21">
-        <f>M6*10^9/M14</f>
+        <f t="shared" si="4"/>
         <v>69.544011143998688</v>
       </c>
       <c r="N21">
-        <f>N6*10^9/N14</f>
+        <f t="shared" si="4"/>
         <v>69.470030019682213</v>
       </c>
       <c r="O21">
-        <f>O6*10^9/O14</f>
+        <f t="shared" si="4"/>
         <v>69.360147792415432</v>
       </c>
       <c r="P21">
-        <f>P6*10^9/P14</f>
+        <f t="shared" si="4"/>
         <v>69.221123931397926</v>
       </c>
       <c r="Q21">
-        <f>Q6*10^9/Q14</f>
+        <f t="shared" si="4"/>
         <v>69.058248470750073</v>
       </c>
       <c r="R21">
-        <f>R6*10^9/R14</f>
+        <f t="shared" si="4"/>
         <v>68.879371981945951</v>
       </c>
       <c r="S21">
-        <f>S6*10^9/S14</f>
+        <f t="shared" si="4"/>
         <v>68.667846073645691</v>
       </c>
       <c r="T21">
-        <f>T6*10^9/T14</f>
+        <f t="shared" si="4"/>
         <v>68.43367051126981</v>
       </c>
       <c r="U21">
-        <f>U6*10^9/U14</f>
+        <f t="shared" si="4"/>
         <v>68.252916178059635</v>
       </c>
       <c r="V21">
-        <f>V6*10^9/V14</f>
+        <f t="shared" si="4"/>
         <v>68.026497687148577</v>
       </c>
       <c r="W21">
-        <f>W6*10^9/W14</f>
+        <f t="shared" si="4"/>
         <v>67.799843553864918</v>
       </c>
       <c r="X21">
-        <f>X6*10^9/X14</f>
+        <f t="shared" si="4"/>
         <v>67.59358241124697</v>
       </c>
       <c r="Y21">
-        <f>Y6*10^9/Y14</f>
+        <f t="shared" si="4"/>
         <v>67.387566640157601</v>
       </c>
       <c r="Z21">
-        <f>Z6*10^9/Z14</f>
+        <f t="shared" si="4"/>
         <v>67.188932192230766</v>
       </c>
       <c r="AA21">
-        <f>AA6*10^9/AA14</f>
+        <f t="shared" si="4"/>
         <v>67.017513659110818</v>
       </c>
       <c r="AB21">
-        <f>AB6*10^9/AB14</f>
+        <f t="shared" si="4"/>
         <v>66.87039437728717</v>
       </c>
       <c r="AC21">
-        <f>AC6*10^9/AC14</f>
+        <f t="shared" si="4"/>
         <v>66.720547173464965</v>
       </c>
       <c r="AD21">
-        <f>AD6*10^9/AD14</f>
+        <f t="shared" si="4"/>
         <v>66.585706298289125</v>
       </c>
       <c r="AE21">
-        <f>AE6*10^9/AE14</f>
+        <f t="shared" si="4"/>
         <v>66.481627933845658</v>
       </c>
       <c r="AF21">
-        <f>AF6*10^9/AF14</f>
+        <f t="shared" si="4"/>
         <v>66.415348433887075</v>
       </c>
       <c r="AG21">
-        <f>AG6*10^9/AG14</f>
+        <f t="shared" si="4"/>
         <v>66.351929151587015</v>
       </c>
       <c r="AH21">
-        <f>AH6*10^9/AH14</f>
+        <f t="shared" si="4"/>
         <v>66.304120262158619</v>
       </c>
       <c r="AI21">
-        <f>AI6*10^9/AI14</f>
+        <f t="shared" si="4"/>
         <v>66.27000008792713</v>
       </c>
       <c r="AJ21">
-        <f>AJ6*10^9/AJ14</f>
+        <f t="shared" si="4"/>
         <v>66.210808181463307</v>
       </c>
       <c r="AK21">
-        <f>AK6*10^9/AK14</f>
+        <f t="shared" si="4"/>
         <v>66.169376509362436</v>
       </c>
       <c r="AL21">
-        <f>AL6*10^9/AL14</f>
+        <f t="shared" si="4"/>
         <v>66.143526887101473</v>
       </c>
       <c r="AM21">
-        <f>AM6*10^9/AM14</f>
+        <f t="shared" si="4"/>
         <v>66.123188380863269</v>
       </c>
       <c r="AN21">
-        <f>AN6*10^9/AN14</f>
+        <f t="shared" si="4"/>
         <v>66.107328337770397</v>
       </c>
       <c r="AO21">
-        <f>AO6*10^9/AO14</f>
+        <f t="shared" si="4"/>
         <v>66.088253495645588</v>
       </c>
     </row>
@@ -4199,159 +4199,159 @@
         <v>101</v>
       </c>
       <c r="C22" t="e">
-        <f>C7*10^9/C15</f>
+        <f t="shared" ref="C22:AO22" si="5">C7*10^9/C15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D22" t="e">
-        <f>D7*10^9/D15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E22" t="e">
-        <f>E7*10^9/E15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F22" t="e">
-        <f>F7*10^9/F15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G22" t="e">
-        <f>G7*10^9/G15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" t="e">
-        <f>H7*10^9/H15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" t="e">
-        <f>I7*10^9/I15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J22" t="e">
-        <f>J7*10^9/J15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" t="e">
-        <f>K7*10^9/K15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L22">
-        <f>L7*10^9/L15</f>
+        <f t="shared" si="5"/>
         <v>60.003331858798532</v>
       </c>
       <c r="M22">
-        <f>M7*10^9/M15</f>
+        <f t="shared" si="5"/>
         <v>59.638670042874104</v>
       </c>
       <c r="N22">
-        <f>N7*10^9/N15</f>
+        <f t="shared" si="5"/>
         <v>59.472406314753989</v>
       </c>
       <c r="O22">
-        <f>O7*10^9/O15</f>
+        <f t="shared" si="5"/>
         <v>58.54414165977073</v>
       </c>
       <c r="P22">
-        <f>P7*10^9/P15</f>
+        <f t="shared" si="5"/>
         <v>57.853882350739234</v>
       </c>
       <c r="Q22">
-        <f>Q7*10^9/Q15</f>
+        <f t="shared" si="5"/>
         <v>57.312366688107275</v>
       </c>
       <c r="R22">
-        <f>R7*10^9/R15</f>
+        <f t="shared" si="5"/>
         <v>56.971866397382726</v>
       </c>
       <c r="S22">
-        <f>S7*10^9/S15</f>
+        <f t="shared" si="5"/>
         <v>56.504900984119551</v>
       </c>
       <c r="T22">
-        <f>T7*10^9/T15</f>
+        <f t="shared" si="5"/>
         <v>56.569706569897697</v>
       </c>
       <c r="U22">
-        <f>U7*10^9/U15</f>
+        <f t="shared" si="5"/>
         <v>56.103933237363087</v>
       </c>
       <c r="V22">
-        <f>V7*10^9/V15</f>
+        <f t="shared" si="5"/>
         <v>56.042893977238904</v>
       </c>
       <c r="W22">
-        <f>W7*10^9/W15</f>
+        <f t="shared" si="5"/>
         <v>55.859693144019033</v>
       </c>
       <c r="X22">
-        <f>X7*10^9/X15</f>
+        <f t="shared" si="5"/>
         <v>55.714422981585365</v>
       </c>
       <c r="Y22">
-        <f>Y7*10^9/Y15</f>
+        <f t="shared" si="5"/>
         <v>55.68147935200659</v>
       </c>
       <c r="Z22">
-        <f>Z7*10^9/Z15</f>
+        <f t="shared" si="5"/>
         <v>55.568694794408025</v>
       </c>
       <c r="AA22">
-        <f>AA7*10^9/AA15</f>
+        <f t="shared" si="5"/>
         <v>55.47189038446853</v>
       </c>
       <c r="AB22">
-        <f>AB7*10^9/AB15</f>
+        <f t="shared" si="5"/>
         <v>55.40382894846325</v>
       </c>
       <c r="AC22">
-        <f>AC7*10^9/AC15</f>
+        <f t="shared" si="5"/>
         <v>55.272005760184122</v>
       </c>
       <c r="AD22">
-        <f>AD7*10^9/AD15</f>
+        <f t="shared" si="5"/>
         <v>55.040968647246345</v>
       </c>
       <c r="AE22">
-        <f>AE7*10^9/AE15</f>
+        <f t="shared" si="5"/>
         <v>55.074990257947853</v>
       </c>
       <c r="AF22">
-        <f>AF7*10^9/AF15</f>
+        <f t="shared" si="5"/>
         <v>55.000152371639835</v>
       </c>
       <c r="AG22">
-        <f>AG7*10^9/AG15</f>
+        <f t="shared" si="5"/>
         <v>54.824201729373399</v>
       </c>
       <c r="AH22">
-        <f>AH7*10^9/AH15</f>
+        <f t="shared" si="5"/>
         <v>54.777902034106475</v>
       </c>
       <c r="AI22">
-        <f>AI7*10^9/AI15</f>
+        <f t="shared" si="5"/>
         <v>54.758066297378519</v>
       </c>
       <c r="AJ22">
-        <f>AJ7*10^9/AJ15</f>
+        <f t="shared" si="5"/>
         <v>54.688603908483913</v>
       </c>
       <c r="AK22">
-        <f>AK7*10^9/AK15</f>
+        <f t="shared" si="5"/>
         <v>54.618857202463197</v>
       </c>
       <c r="AL22">
-        <f>AL7*10^9/AL15</f>
+        <f t="shared" si="5"/>
         <v>54.614176388106344</v>
       </c>
       <c r="AM22">
-        <f>AM7*10^9/AM15</f>
+        <f t="shared" si="5"/>
         <v>54.591434883340682</v>
       </c>
       <c r="AN22">
-        <f>AN7*10^9/AN15</f>
+        <f t="shared" si="5"/>
         <v>54.561393345673501</v>
       </c>
       <c r="AO22">
-        <f>AO7*10^9/AO15</f>
+        <f t="shared" si="5"/>
         <v>54.550898106764869</v>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
   <dimension ref="A1:AO70"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8849,16 +8849,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <f>savings_residential!U30</f>
-        <v>-0.2982701080862078</v>
+        <f>savings_residential!U30*-1</f>
+        <v>0.2982701080862078</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" ref="C2:C7" si="0">$B2</f>
-        <v>-0.2982701080862078</v>
+        <v>0.2982701080862078</v>
       </c>
       <c r="D2" s="7">
-        <f>savings_commercial!U31</f>
-        <v>-0.1894572490022555</v>
+        <f>savings_commercial!U27*-1</f>
+        <v>0.21716157980901149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -8867,15 +8867,15 @@
       </c>
       <c r="B3" s="7">
         <f>B2</f>
-        <v>-0.2982701080862078</v>
+        <v>0.2982701080862078</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
-        <v>-0.2982701080862078</v>
+        <v>0.2982701080862078</v>
       </c>
       <c r="D3" s="7">
         <f>D2</f>
-        <v>-0.1894572490022555</v>
+        <v>0.21716157980901149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -9077,6 +9077,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9085,7 +9096,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4a12692b057bc30d68596ac87c75a308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd464ebbb7361a2027b4bc4be8d527a" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -9314,18 +9325,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16BCF5D9-3972-43CF-88C7-BA42C2BD5A61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCF26DFC-E322-4B03-BD33-D84AE438B047}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9333,7 +9344,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923BB36F-34B4-48B9-A841-D5CFBCACFD83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9350,15 +9361,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16BCF5D9-3972-43CF-88C7-BA42C2BD5A61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated retrofitting to a smaller portion of buildings at a more aggressive rate
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BRESaC/Bldg Retrofitting E Savings and Costs.xlsx
+++ b/InputData/bldgs/BRESaC/Bldg Retrofitting E Savings and Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\bldgs\BRESaC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\bldgs\BRESaC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE871DA-E75B-4A5D-8918-0BDE2A174455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2692DF89-CEEC-4EFD-A5B2-F3E9DCD3779B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33105" yWindow="3045" windowWidth="18765" windowHeight="12960" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="122">
   <si>
     <t>BRESaC Percent Energy Savings from Retrofitting by Component</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>Share of bldg floorspace from pre 1961 and 1961-90</t>
+  </si>
+  <si>
+    <t>Share of bldg floorspace from pre 1961</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +504,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,7 +585,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,6 +628,9 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1971,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995D26CD-6318-4B74-895D-30922EB64AE0}">
-  <dimension ref="A1:AO61"/>
+  <dimension ref="A1:AO64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2742,160 +2754,160 @@
         <v>103</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:AO8" si="0">SUM(C4:C7)</f>
-        <v>535.38849971629782</v>
+        <f>SUM(C3:C7)</f>
+        <v>796.02743900576957</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>538.91909208493371</v>
+        <f t="shared" ref="D8:AO8" si="0">SUM(D3:D7)</f>
+        <v>795.19596136539224</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>543.29009945444216</v>
+        <v>795.36882514207798</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>546.7204540729299</v>
+        <v>794.60559318703793</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>549.28457075994061</v>
+        <v>793.04525758054388</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>555.29806501142377</v>
+        <v>794.9649949870111</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>555.23738279998452</v>
+        <v>790.82416001457432</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>556.8732893557135</v>
+        <v>788.46536446164635</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>554.0278424429348</v>
+        <v>781.59228663375347</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>550.56783194589127</v>
+        <v>773.86901493211951</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>548.37493747815552</v>
+        <v>767.55151384503029</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>544.99710395265561</v>
+        <v>759.93282837839422</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>542.18381433119214</v>
+        <v>752.96598378954002</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>541.19772315441071</v>
+        <v>747.87323110300053</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>538.82420337273811</v>
+        <v>741.58820753767372</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>536.90178990782317</v>
+        <v>735.72744478637617</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>535.63580402753439</v>
+        <v>730.7036297073746</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>534.08076165051421</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="0"/>
-        <v>532.56628229455873</v>
+        <v>725.36663489329339</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>720.13628524414344</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>530.03536899271614</v>
+        <v>713.97894260463602</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>527.97466379714001</v>
+        <v>708.28700372299011</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>525.71982441055434</v>
+        <v>702.56314369062113</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>523.36160076869703</v>
-      </c>
-      <c r="Z8" s="1">
-        <f t="shared" si="0"/>
-        <v>521.23944186205233</v>
+        <v>696.83645554550264</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>691.41887576561987</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>518.47030630453719</v>
+        <v>685.35959063109499</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>516.16058222964398</v>
+        <v>679.88670426760677</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>513.29215901858265</v>
+        <v>673.94711222636602</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>510.637454684668</v>
+        <v>668.31985805803993</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>508.01872211266925</v>
+        <v>662.78531892700721</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>505.17939508129223</v>
+        <v>657.08440078492686</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>502.91324698355646</v>
+        <v>652.0531495420023</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>500.24822351918971</v>
+        <v>646.60880202617705</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>497.58427326763183</v>
+        <v>641.27354358024377</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>495.3581814188214</v>
+        <v>636.47987975172703</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>492.23946501319421</v>
+        <v>630.8549761903995</v>
       </c>
       <c r="AL8">
         <f t="shared" si="0"/>
-        <v>489.56765175759978</v>
+        <v>625.70384343039757</v>
       </c>
       <c r="AM8">
         <f t="shared" si="0"/>
-        <v>486.76362275995768</v>
+        <v>620.40262946281666</v>
       </c>
       <c r="AN8">
         <f t="shared" si="0"/>
-        <v>485.02267708619758</v>
+        <v>616.33128117371791</v>
       </c>
       <c r="AO8">
         <f t="shared" si="0"/>
-        <v>482.66195114430155</v>
+        <v>611.6849402133189</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.35">
@@ -3530,16 +3542,16 @@
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="T16" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="U16" s="29">
-        <f>SUM(U11:U12)/SUM(U11:U15)</f>
-        <v>0.49892341517071065</v>
+        <f>SUM(U11)/SUM(U11:U14)</f>
+        <v>0.25299594354555016</v>
       </c>
       <c r="V16" s="27"/>
       <c r="Z16" s="27">
-        <f>SUM(Z11:Z12)/SUM(Z11:Z15)</f>
-        <v>0.46277867078299695</v>
+        <f>SUM(Z11)/SUM(Z11:Z14)</f>
+        <v>0.25321691235952715</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.35">
@@ -4388,16 +4400,16 @@
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
       <c r="U26" s="29">
-        <f>(U20-U18)/U18</f>
-        <v>-0.15376422553044544</v>
+        <f>(U21-U18)/U18</f>
+        <v>-0.5054597997188619</v>
       </c>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="24"/>
       <c r="Y26" s="24"/>
       <c r="Z26" s="29">
-        <f>(Z20-Z18)/Z18</f>
-        <v>-0.11618508340611038</v>
+        <f>(Z21-Z18)/Z18</f>
+        <v>-0.48228657644735579</v>
       </c>
       <c r="AA26" s="24"/>
     </row>
@@ -4426,15 +4438,15 @@
       <c r="R27" s="24"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
-      <c r="U27" s="29">
+      <c r="U27" s="32">
         <f>(U20-U19)/U19</f>
         <v>-0.21716157980901149</v>
       </c>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="29">
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="33"/>
+      <c r="Z27" s="32">
         <f>(Z20-Z19)/Z19</f>
         <v>-0.19550366112122455</v>
       </c>
@@ -4542,21 +4554,21 @@
     <row r="31" spans="1:41" x14ac:dyDescent="0.35">
       <c r="U31" s="30">
         <f>(U26*U11+U27*U12)/SUM(U11:U12)</f>
-        <v>-0.1894572490022555</v>
+        <v>-0.34314647848926666</v>
       </c>
       <c r="Z31" s="30">
         <f>(Z26*Z11+Z27*Z12)/SUM(Z11:Z12)</f>
-        <v>-0.1606554420496199</v>
+        <v>-0.3215002957958038</v>
       </c>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.35">
       <c r="U34" s="31">
-        <f>SUM(U11:U12)/SUM(U11:U14)</f>
-        <v>0.5789446269565186</v>
+        <f>SUM(U11)/SUM(U11:U14)</f>
+        <v>0.25299594354555016</v>
       </c>
       <c r="Z34" s="31">
-        <f>SUM(Z11:Z12)/SUM(Z11:Z14)</f>
-        <v>0.57635098369018545</v>
+        <f>SUM(Z11)/SUM(Z11:Z14)</f>
+        <v>0.25321691235952715</v>
       </c>
     </row>
     <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
@@ -4774,7 +4786,7 @@
       </c>
       <c r="U46" s="18">
         <f>U8-U44</f>
-        <v>48.957227678273284</v>
+        <v>236.52723062785799</v>
       </c>
       <c r="V46" t="s">
         <v>38</v>
@@ -4784,7 +4796,7 @@
       </c>
       <c r="Z46" s="18">
         <f>Z8-Z44</f>
-        <v>38.044887129072436</v>
+        <v>208.22432103263998</v>
       </c>
       <c r="AA46" t="s">
         <v>38</v>
@@ -4796,14 +4808,14 @@
       </c>
       <c r="U47" s="19">
         <f>U46/U8</f>
-        <v>9.1927013229867557E-2</v>
+        <v>0.32844787226305311</v>
       </c>
       <c r="Y47" s="16" t="s">
         <v>110</v>
       </c>
       <c r="Z47" s="19">
         <f>Z46/Z8</f>
-        <v>7.2989271481763915E-2</v>
+        <v>0.30115510052002797</v>
       </c>
     </row>
     <row r="48" spans="1:41" hidden="1" x14ac:dyDescent="0.35"/>
@@ -4978,7 +4990,7 @@
       </c>
       <c r="U60" s="22">
         <f>U8-U58</f>
-        <v>-101.9999467190712</v>
+        <v>85.570056230513501</v>
       </c>
       <c r="V60" t="s">
         <v>38</v>
@@ -4988,7 +5000,7 @@
       </c>
       <c r="Z60" s="22">
         <f>Z8-Z58</f>
-        <v>-103.76382228533646</v>
+        <v>66.415611618231083</v>
       </c>
       <c r="AA60" t="s">
         <v>38</v>
@@ -5000,14 +5012,34 @@
       </c>
       <c r="U61" s="23">
         <f>U60/U8</f>
-        <v>-0.19152535582914679</v>
+        <v>0.11882480855898436</v>
       </c>
       <c r="Y61" s="21" t="s">
         <v>110</v>
       </c>
       <c r="Z61" s="23">
         <f>Z60/Z8</f>
-        <v>-0.19907131723312274</v>
+        <v>9.6056983611689725E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="U63" s="34">
+        <f>SUM(U4:U7)+(U3*(1+U26))</f>
+        <v>625.32718911998006</v>
+      </c>
+      <c r="Z63" s="34">
+        <f>SUM(Z4:Z7)+(Z3*(1+Z26))</f>
+        <v>609.34361920651918</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="U64" s="27">
+        <f>(U8-U63)/U8</f>
+        <v>0.13165437996506568</v>
+      </c>
+      <c r="Z64" s="27">
+        <f>(Z8-Z63)/Z8</f>
+        <v>0.11870554801995732</v>
       </c>
     </row>
   </sheetData>
@@ -5019,15 +5051,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A9921B-F39F-43F4-ABB5-C04C9CADE685}">
   <dimension ref="A1:AO70"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="19" width="12.54296875" hidden="1" customWidth="1"/>
-    <col min="20" max="41" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="41" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.35">
@@ -6581,13 +6615,13 @@
         <v>120</v>
       </c>
       <c r="U16" s="29">
-        <f>SUM(U11:U12)/SUM(U11:U15)</f>
-        <v>0.61339818239717359</v>
+        <f>SUM(U11)/SUM(U11:U14)</f>
+        <v>0.30293549821580473</v>
       </c>
       <c r="V16" s="27"/>
       <c r="Z16" s="27">
-        <f>SUM(Z11:Z12)/SUM(Z11:Z15)</f>
-        <v>0.59473241797358878</v>
+        <f>SUM(Z11)/SUM(Z11:Z14)</f>
+        <v>0.30228767126214501</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.35">
@@ -7430,16 +7464,16 @@
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="U25" s="29">
-        <f>(U20-U18)/U18</f>
-        <v>-0.26423984800049788</v>
+        <f>(U21-U18)/U18</f>
+        <v>-0.74057464160058584</v>
       </c>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
       <c r="Y25" s="24"/>
       <c r="Z25" s="29">
-        <f>(Z20-Z18)/Z18</f>
-        <v>-0.24189102980113422</v>
+        <f>(Z21-Z18)/Z18</f>
+        <v>-0.72793852335316056</v>
       </c>
       <c r="AA25" s="24"/>
       <c r="AB25" s="24"/>
@@ -7482,15 +7516,15 @@
       <c r="R26" s="24"/>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
-      <c r="U26" s="29">
+      <c r="U26" s="32">
         <f>(U20-U19)/U19</f>
         <v>-0.32742324978842557</v>
       </c>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="29">
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="33"/>
+      <c r="Z26" s="32">
         <f>(Z20-Z19)/Z19</f>
         <v>-0.31492114692229495</v>
       </c>
@@ -7654,11 +7688,11 @@
     <row r="30" spans="1:41" x14ac:dyDescent="0.35">
       <c r="U30" s="30">
         <f>(U25*U11+U26*U12)/SUM(U11:U12)</f>
-        <v>-0.2982701080862078</v>
+        <v>-0.51805339519268512</v>
       </c>
       <c r="Z30" s="30">
         <f>(Z25*Z11+Z26*Z12)/SUM(Z11:Z12)</f>
-        <v>-0.28127354749345396</v>
+        <v>-0.50521309478047327</v>
       </c>
     </row>
     <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.35">
@@ -8317,12 +8351,12 @@
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.35">
       <c r="U38" s="31">
-        <f>SUM(U11:U12)/SUM(U11:U14)</f>
-        <v>0.65655000394482876</v>
+        <f>SUM(U11)/SUM(U11:U14)</f>
+        <v>0.30293549821580473</v>
       </c>
       <c r="Z38" s="31">
-        <f>SUM(Z11:Z12)/SUM(Z11:Z14)</f>
-        <v>0.6560974456214822</v>
+        <f>SUM(Z11)/SUM(Z11:Z14)</f>
+        <v>0.30228767126214501</v>
       </c>
     </row>
     <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.35"/>
@@ -8779,23 +8813,23 @@
       </c>
     </row>
     <row r="66" spans="21:26" x14ac:dyDescent="0.35">
-      <c r="U66">
-        <f>U8*U16*(1-U30)</f>
-        <v>1387.1046351868599</v>
-      </c>
-      <c r="Z66">
-        <f>Z8*Z16*(1-Z30)</f>
-        <v>1259.336773626088</v>
+      <c r="U66" s="34">
+        <f>SUM(U4:U7)+(U3*(1+U25))</f>
+        <v>1309.9773809344986</v>
+      </c>
+      <c r="Z66" s="34">
+        <f>SUM(Z4:Z7)+(Z3*(1+Z25))</f>
+        <v>1257.3882781611842</v>
       </c>
     </row>
     <row r="67" spans="21:26" x14ac:dyDescent="0.35">
       <c r="U67" s="27">
         <f>(U8-U66)/U8</f>
-        <v>0.203643475439338</v>
+        <v>0.24792333046054402</v>
       </c>
       <c r="Z67" s="27">
         <f>(Z8-Z66)/Z8</f>
-        <v>0.23798508501362034</v>
+        <v>0.23916410450795683</v>
       </c>
     </row>
     <row r="69" spans="21:26" x14ac:dyDescent="0.35">
@@ -8818,8 +8852,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8849,16 +8883,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <f>savings_residential!U30*-1</f>
-        <v>0.2982701080862078</v>
+        <f>savings_residential!U25*-1</f>
+        <v>0.74057464160058584</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" ref="C2:C7" si="0">$B2</f>
-        <v>0.2982701080862078</v>
+        <v>0.74057464160058584</v>
       </c>
       <c r="D2" s="7">
-        <f>savings_commercial!U27*-1</f>
-        <v>0.21716157980901149</v>
+        <f>savings_commercial!U26*-1</f>
+        <v>0.5054597997188619</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -8867,15 +8901,15 @@
       </c>
       <c r="B3" s="7">
         <f>B2</f>
-        <v>0.2982701080862078</v>
+        <v>0.74057464160058584</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
-        <v>0.2982701080862078</v>
+        <v>0.74057464160058584</v>
       </c>
       <c r="D3" s="7">
         <f>D2</f>
-        <v>0.21716157980901149</v>
+        <v>0.5054597997188619</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -9088,15 +9122,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4a12692b057bc30d68596ac87c75a308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd464ebbb7361a2027b4bc4be8d527a" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -9325,6 +9350,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16BCF5D9-3972-43CF-88C7-BA42C2BD5A61}">
   <ds:schemaRefs>
@@ -9337,14 +9371,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCF26DFC-E322-4B03-BD33-D84AE438B047}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923BB36F-34B4-48B9-A841-D5CFBCACFD83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9361,4 +9387,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCF26DFC-E322-4B03-BD33-D84AE438B047}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>